<commit_message>
Add new sample xlsx file
</commit_message>
<xml_diff>
--- a/TWEAC_MI100_Instruction_Roofline_Metrics.xlsx
+++ b/TWEAC_MI100_Instruction_Roofline_Metrics.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewleinhauser/Library/Mobile Documents/com~apple~CloudDocs/Research/TWEAC/AMD Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C746E9-E0B4-8D4D-9C58-519205E4149A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9614321-6839-114F-A153-6ACCF6880B62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NewTWEAC_MI100_Instruction_Roof" sheetId="1" r:id="rId1"/>
+    <sheet name="tweac_mi100_rocProf_metrics_Mar" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="30">
   <si>
     <t>Index</t>
   </si>
@@ -93,9 +93,6 @@
     <t>SQ_INSTS_SALU</t>
   </si>
   <si>
-    <t>GPUBusy</t>
-  </si>
-  <si>
     <t>BeginNs</t>
   </si>
   <si>
@@ -105,10 +102,10 @@
     <t>0x0</t>
   </si>
   <si>
-    <t>0x15512927fb80</t>
-  </si>
-  <si>
-    <t>0x155129281180</t>
+    <t>0x15512b27eec0</t>
+  </si>
+  <si>
+    <t>0x15512b2804c0</t>
   </si>
   <si>
     <t>MoveAndMark</t>
@@ -618,9 +615,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -976,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -990,25 +987,24 @@
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.5" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1075,22 +1071,19 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="5" t="s">
+      <c r="W1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="5" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>870</v>
+        <v>924</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1099,16 +1092,16 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>1304</v>
+        <v>1438</v>
       </c>
       <c r="F2">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G2">
-        <v>756446</v>
+        <v>388986</v>
       </c>
       <c r="H2">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I2">
         <v>256</v>
@@ -1123,53 +1116,50 @@
         <v>56</v>
       </c>
       <c r="M2">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N2">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q2">
-        <v>1626553</v>
+        <v>11460394</v>
       </c>
       <c r="R2">
-        <v>1857650532</v>
+        <v>14496863558</v>
       </c>
       <c r="S2">
-        <v>82927</v>
+        <v>792172</v>
       </c>
       <c r="T2">
-        <v>676498269</v>
-      </c>
-      <c r="U2">
-        <v>100</v>
-      </c>
-      <c r="V2">
-        <v>500848137652881</v>
-      </c>
-      <c r="W2">
-        <v>500848159086726</v>
-      </c>
-      <c r="X2" s="6">
-        <f>W2-V2</f>
-        <v>21433845</v>
-      </c>
-      <c r="Y2">
-        <f>X2 * POWER(10, -9)</f>
-        <v>2.1433845E-2</v>
+        <v>5250476445</v>
+      </c>
+      <c r="U2" s="4">
+        <v>267573387119164</v>
+      </c>
+      <c r="V2" s="4">
+        <v>267573553232839</v>
+      </c>
+      <c r="W2" s="4">
+        <f>V2-U2</f>
+        <v>166113675</v>
+      </c>
+      <c r="X2">
+        <f>W2 * POWER(10, -9)</f>
+        <v>0.16611367500000002</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1254</v>
+        <v>1361</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1178,16 +1168,16 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <v>334</v>
+        <v>351</v>
       </c>
       <c r="F3">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G3">
-        <v>756457</v>
+        <v>388997</v>
       </c>
       <c r="H3">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I3">
         <v>256</v>
@@ -1202,71 +1192,68 @@
         <v>56</v>
       </c>
       <c r="M3">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N3">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q3">
-        <v>1624316</v>
+        <v>11424106</v>
       </c>
       <c r="R3">
-        <v>2180889918</v>
+        <v>17460883906</v>
       </c>
       <c r="S3">
-        <v>71351</v>
+        <v>758642</v>
       </c>
       <c r="T3">
-        <v>892176606</v>
-      </c>
-      <c r="U3">
-        <v>100</v>
-      </c>
-      <c r="V3">
-        <v>500848306505723</v>
-      </c>
-      <c r="W3">
-        <v>500848335581461</v>
-      </c>
-      <c r="X3" s="6">
-        <f t="shared" ref="X3:X22" si="0">W3-V3</f>
-        <v>29075738</v>
-      </c>
-      <c r="Y3">
-        <f t="shared" ref="Y3:Y22" si="1">X3 * POWER(10, -9)</f>
-        <v>2.9075738E-2</v>
+        <v>7227789925</v>
+      </c>
+      <c r="U3" s="4">
+        <v>267574113519421</v>
+      </c>
+      <c r="V3" s="4">
+        <v>267574380456932</v>
+      </c>
+      <c r="W3" s="4">
+        <f t="shared" ref="W3:W22" si="0">V3-U3</f>
+        <v>266937511</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X23" si="1">W3 * POWER(10, -9)</f>
+        <v>0.26693751100000002</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1638</v>
+        <v>1797</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>1669</v>
+        <v>550</v>
       </c>
       <c r="F4">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G4">
-        <v>756455</v>
+        <v>388994</v>
       </c>
       <c r="H4">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I4">
         <v>256</v>
@@ -1281,71 +1268,68 @@
         <v>56</v>
       </c>
       <c r="M4">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N4">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q4">
-        <v>1624136</v>
+        <v>11373732</v>
       </c>
       <c r="R4">
-        <v>2205629044</v>
+        <v>16822204058</v>
       </c>
       <c r="S4">
-        <v>70608</v>
+        <v>652977</v>
       </c>
       <c r="T4">
-        <v>908521326</v>
-      </c>
-      <c r="U4">
-        <v>100</v>
-      </c>
-      <c r="V4">
-        <v>500848476623022</v>
-      </c>
-      <c r="W4">
-        <v>500848506720676</v>
-      </c>
-      <c r="X4" s="6">
+        <v>6801251914</v>
+      </c>
+      <c r="U4" s="4">
+        <v>267574903415811</v>
+      </c>
+      <c r="V4" s="4">
+        <v>267575126127367</v>
+      </c>
+      <c r="W4" s="4">
         <f t="shared" si="0"/>
-        <v>30097654</v>
-      </c>
-      <c r="Y4">
+        <v>222711556</v>
+      </c>
+      <c r="X4">
         <f t="shared" si="1"/>
-        <v>3.0097654000000001E-2</v>
+        <v>0.222711556</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2022</v>
+        <v>2234</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>695</v>
+        <v>2098</v>
       </c>
       <c r="F5">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G5">
-        <v>756453</v>
+        <v>388986</v>
       </c>
       <c r="H5">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I5">
         <v>256</v>
@@ -1360,71 +1344,68 @@
         <v>56</v>
       </c>
       <c r="M5">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N5">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q5">
-        <v>1624185</v>
+        <v>11375982</v>
       </c>
       <c r="R5">
-        <v>2213347125</v>
+        <v>17684195069</v>
       </c>
       <c r="S5">
-        <v>72826</v>
+        <v>721048</v>
       </c>
       <c r="T5">
-        <v>913900028</v>
-      </c>
-      <c r="U5">
-        <v>100</v>
-      </c>
-      <c r="V5">
-        <v>500848648574329</v>
-      </c>
-      <c r="W5">
-        <v>500848679260623</v>
-      </c>
-      <c r="X5" s="6">
+        <v>7376159687</v>
+      </c>
+      <c r="U5" s="4">
+        <v>267575677359131</v>
+      </c>
+      <c r="V5" s="4">
+        <v>267575926355643</v>
+      </c>
+      <c r="W5" s="4">
         <f t="shared" si="0"/>
-        <v>30686294</v>
-      </c>
-      <c r="Y5">
+        <v>248996512</v>
+      </c>
+      <c r="X5">
         <f t="shared" si="1"/>
-        <v>3.0686294000000003E-2</v>
+        <v>0.248996512</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2406</v>
+        <v>2671</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>883</v>
+        <v>1000</v>
       </c>
       <c r="F6">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G6">
-        <v>756458</v>
+        <v>388997</v>
       </c>
       <c r="H6">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I6">
         <v>256</v>
@@ -1439,71 +1420,68 @@
         <v>56</v>
       </c>
       <c r="M6">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N6">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q6">
-        <v>1624065</v>
+        <v>11371429</v>
       </c>
       <c r="R6">
-        <v>2219835710</v>
+        <v>17162195132</v>
       </c>
       <c r="S6">
-        <v>71371</v>
+        <v>696764</v>
       </c>
       <c r="T6">
-        <v>918407082</v>
-      </c>
-      <c r="U6">
-        <v>93</v>
-      </c>
-      <c r="V6">
-        <v>500848848944144</v>
-      </c>
-      <c r="W6">
-        <v>500848880095876</v>
-      </c>
-      <c r="X6" s="6">
+        <v>7028640447</v>
+      </c>
+      <c r="U6" s="4">
+        <v>267576450069249</v>
+      </c>
+      <c r="V6" s="4">
+        <v>267576683779775</v>
+      </c>
+      <c r="W6" s="4">
         <f t="shared" si="0"/>
-        <v>31151732</v>
-      </c>
-      <c r="Y6">
+        <v>233710526</v>
+      </c>
+      <c r="X6">
         <f t="shared" si="1"/>
-        <v>3.1151732000000001E-2</v>
+        <v>0.233710526</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2791</v>
+        <v>3107</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>1084</v>
+        <v>1182</v>
       </c>
       <c r="F7">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G7">
-        <v>756457</v>
+        <v>388994</v>
       </c>
       <c r="H7">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I7">
         <v>256</v>
@@ -1518,71 +1496,68 @@
         <v>56</v>
       </c>
       <c r="M7">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N7">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q7">
-        <v>1623947</v>
+        <v>11373941</v>
       </c>
       <c r="R7">
-        <v>2225651586</v>
+        <v>17764624449</v>
       </c>
       <c r="S7">
-        <v>72528</v>
+        <v>724327</v>
       </c>
       <c r="T7">
-        <v>922283547</v>
-      </c>
-      <c r="U7">
-        <v>100</v>
-      </c>
-      <c r="V7">
-        <v>500849033464729</v>
-      </c>
-      <c r="W7">
-        <v>500849065004778</v>
-      </c>
-      <c r="X7" s="6">
+        <v>7430073024</v>
+      </c>
+      <c r="U7" s="4">
+        <v>267577315575294</v>
+      </c>
+      <c r="V7" s="4">
+        <v>267577564167971</v>
+      </c>
+      <c r="W7" s="4">
         <f t="shared" si="0"/>
-        <v>31540049</v>
-      </c>
-      <c r="Y7">
+        <v>248592677</v>
+      </c>
+      <c r="X7">
         <f t="shared" si="1"/>
-        <v>3.1540049000000001E-2</v>
+        <v>0.24859267700000001</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>3175</v>
+        <v>3543</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>2421</v>
+        <v>1404</v>
       </c>
       <c r="F8">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G8">
-        <v>756455</v>
+        <v>388998</v>
       </c>
       <c r="H8">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I8">
         <v>256</v>
@@ -1597,71 +1572,68 @@
         <v>56</v>
       </c>
       <c r="M8">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N8">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>1624111</v>
+        <v>11416152</v>
       </c>
       <c r="R8">
-        <v>2231173336</v>
+        <v>17413214080</v>
       </c>
       <c r="S8">
-        <v>72497</v>
+        <v>712262</v>
       </c>
       <c r="T8">
-        <v>925606448</v>
-      </c>
-      <c r="U8">
-        <v>100</v>
-      </c>
-      <c r="V8">
-        <v>500849206003731</v>
-      </c>
-      <c r="W8">
-        <v>500849237822501</v>
-      </c>
-      <c r="X8" s="6">
+        <v>7196306654</v>
+      </c>
+      <c r="U8" s="4">
+        <v>267578183161712</v>
+      </c>
+      <c r="V8" s="4">
+        <v>267578452328176</v>
+      </c>
+      <c r="W8" s="4">
         <f t="shared" si="0"/>
-        <v>31818770</v>
-      </c>
-      <c r="Y8">
+        <v>269166464</v>
+      </c>
+      <c r="X8">
         <f t="shared" si="1"/>
-        <v>3.1818770000000003E-2</v>
+        <v>0.26916646399999999</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3560</v>
+        <v>3980</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1406</v>
+        <v>799</v>
       </c>
       <c r="F9">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G9">
-        <v>756454</v>
+        <v>388996</v>
       </c>
       <c r="H9">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I9">
         <v>256</v>
@@ -1676,71 +1648,68 @@
         <v>56</v>
       </c>
       <c r="M9">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N9">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9">
-        <v>1623946</v>
+        <v>11413252</v>
       </c>
       <c r="R9">
-        <v>2236022801</v>
+        <v>17701107562</v>
       </c>
       <c r="S9">
-        <v>72994</v>
+        <v>655153</v>
       </c>
       <c r="T9">
-        <v>928888366</v>
-      </c>
-      <c r="U9">
-        <v>100</v>
-      </c>
-      <c r="V9">
-        <v>500849419906276</v>
-      </c>
-      <c r="W9">
-        <v>500849451952406</v>
-      </c>
-      <c r="X9" s="6">
+        <v>7387753189</v>
+      </c>
+      <c r="U9" s="4">
+        <v>267579032796147</v>
+      </c>
+      <c r="V9" s="4">
+        <v>267579302007573</v>
+      </c>
+      <c r="W9" s="4">
         <f t="shared" si="0"/>
-        <v>32046130</v>
-      </c>
-      <c r="Y9">
+        <v>269211426</v>
+      </c>
+      <c r="X9">
         <f t="shared" si="1"/>
-        <v>3.2046129999999999E-2</v>
+        <v>0.26921142600000003</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>3945</v>
+        <v>4418</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>1646</v>
+        <v>3168</v>
       </c>
       <c r="F10">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G10">
-        <v>756453</v>
+        <v>388995</v>
       </c>
       <c r="H10">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I10">
         <v>256</v>
@@ -1755,71 +1724,68 @@
         <v>56</v>
       </c>
       <c r="M10">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N10">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q10">
-        <v>1623847</v>
+        <v>11412551</v>
       </c>
       <c r="R10">
-        <v>2239972639</v>
+        <v>17562296063</v>
       </c>
       <c r="S10">
-        <v>121361</v>
+        <v>720847</v>
       </c>
       <c r="T10">
-        <v>932538647</v>
-      </c>
-      <c r="U10">
-        <v>100</v>
-      </c>
-      <c r="V10">
-        <v>500849600755657</v>
-      </c>
-      <c r="W10">
-        <v>500849632963226</v>
-      </c>
-      <c r="X10" s="6">
+        <v>7295828995</v>
+      </c>
+      <c r="U10" s="4">
+        <v>267579858066100</v>
+      </c>
+      <c r="V10" s="4">
+        <v>267580128285514</v>
+      </c>
+      <c r="W10" s="4">
         <f t="shared" si="0"/>
-        <v>32207569</v>
-      </c>
-      <c r="Y10">
+        <v>270219414</v>
+      </c>
+      <c r="X10">
         <f t="shared" si="1"/>
-        <v>3.2207569000000005E-2</v>
+        <v>0.27021941399999999</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>4328</v>
+        <v>4854</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>1814</v>
+        <v>3395</v>
       </c>
       <c r="F11">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G11">
-        <v>756457</v>
+        <v>388986</v>
       </c>
       <c r="H11">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I11">
         <v>256</v>
@@ -1834,104 +1800,99 @@
         <v>56</v>
       </c>
       <c r="M11">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N11">
-        <v>319808</v>
+        <v>332800</v>
       </c>
       <c r="O11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11">
+        <v>11409464</v>
+      </c>
+      <c r="R11">
+        <v>17347239055</v>
+      </c>
+      <c r="S11">
+        <v>703735</v>
+      </c>
+      <c r="T11">
+        <v>7151505958</v>
+      </c>
+      <c r="U11" s="4">
+        <v>267580677778966</v>
+      </c>
+      <c r="V11" s="4">
+        <v>267580938154917</v>
+      </c>
+      <c r="W11" s="4">
+        <f t="shared" si="0"/>
+        <v>260375951</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="1"/>
+        <v>0.26037595099999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="3">
+        <f>MAX(Q2:Q11)</f>
+        <v>11460394</v>
+      </c>
+      <c r="R12" s="3">
+        <f t="shared" ref="R12:T12" si="2">MAX(R2:R11)</f>
+        <v>17764624449</v>
+      </c>
+      <c r="S12" s="3">
+        <f t="shared" si="2"/>
+        <v>792172</v>
+      </c>
+      <c r="T12" s="3">
+        <f t="shared" si="2"/>
+        <v>7430073024</v>
+      </c>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5">
+        <f>AVERAGE(W2:W11)</f>
+        <v>245603571.19999999</v>
+      </c>
+      <c r="X12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.24560357120000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>755</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q11">
-        <v>1623874</v>
-      </c>
-      <c r="R11">
-        <v>2243681391</v>
-      </c>
-      <c r="S11">
-        <v>73573</v>
-      </c>
-      <c r="T11">
-        <v>934079591</v>
-      </c>
-      <c r="U11">
-        <v>100</v>
-      </c>
-      <c r="V11">
-        <v>500849778560307</v>
-      </c>
-      <c r="W11">
-        <v>500849810839714</v>
-      </c>
-      <c r="X11" s="6">
-        <f t="shared" si="0"/>
-        <v>32279407</v>
-      </c>
-      <c r="Y11">
-        <f t="shared" si="1"/>
-        <v>3.2279407000000003E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q12" s="3">
-        <f>AVERAGE(Q2:Q11)</f>
-        <v>1624298</v>
-      </c>
-      <c r="R12" s="3">
-        <f>AVERAGE(R2:R11)</f>
-        <v>2185385408.1999998</v>
-      </c>
-      <c r="S12" s="3">
-        <f>AVERAGE(S2:S11)</f>
-        <v>78203.600000000006</v>
-      </c>
-      <c r="T12" s="3">
-        <f>AVERAGE(T2:T11)</f>
-        <v>895289991</v>
-      </c>
-      <c r="U12" s="4">
-        <f>AVERAGE(U2:U11)</f>
-        <v>99.3</v>
-      </c>
-      <c r="X12" s="4">
-        <f>AVERAGE(X2:X11)</f>
-        <v>30233718.800000001</v>
-      </c>
-      <c r="Y12" s="3">
-        <f t="shared" si="1"/>
-        <v>3.0233718800000003E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>703</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>68</v>
+        <v>1336</v>
       </c>
       <c r="F13">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G13">
-        <v>756457</v>
+        <v>388995</v>
       </c>
       <c r="H13">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I13">
         <v>256</v>
@@ -1940,77 +1901,74 @@
         <v>28160</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L13">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M13">
         <v>112</v>
       </c>
       <c r="N13">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" t="s">
         <v>23</v>
       </c>
-      <c r="P13" t="s">
-        <v>24</v>
-      </c>
       <c r="Q13">
-        <v>1667106</v>
+        <v>11759321</v>
       </c>
       <c r="R13">
-        <v>1030876869</v>
+        <v>7425910936</v>
       </c>
       <c r="S13">
-        <v>1389463</v>
+        <v>11594515</v>
       </c>
       <c r="T13">
-        <v>57351688</v>
-      </c>
-      <c r="U13">
-        <v>100</v>
-      </c>
-      <c r="V13">
-        <v>500848065420275</v>
-      </c>
-      <c r="W13">
-        <v>500848079167905</v>
-      </c>
-      <c r="X13" s="6">
+        <v>145895567</v>
+      </c>
+      <c r="U13" s="4">
+        <v>267572987827946</v>
+      </c>
+      <c r="V13" s="4">
+        <v>267573148469327</v>
+      </c>
+      <c r="W13" s="4">
         <f t="shared" si="0"/>
-        <v>13747630</v>
-      </c>
-      <c r="Y13">
+        <v>160641381</v>
+      </c>
+      <c r="X13">
         <f t="shared" si="1"/>
-        <v>1.374763E-2</v>
+        <v>0.160641381</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1086</v>
+        <v>1191</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>254</v>
+        <v>1563</v>
       </c>
       <c r="F14">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G14">
-        <v>756454</v>
+        <v>388986</v>
       </c>
       <c r="H14">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I14">
         <v>256</v>
@@ -2019,77 +1977,74 @@
         <v>28160</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L14">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M14">
         <v>112</v>
       </c>
       <c r="N14">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O14" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" t="s">
         <v>23</v>
       </c>
-      <c r="P14" t="s">
-        <v>24</v>
-      </c>
       <c r="Q14">
-        <v>1668951</v>
+        <v>11732737</v>
       </c>
       <c r="R14">
-        <v>1035789431</v>
+        <v>7461005616</v>
       </c>
       <c r="S14">
-        <v>1393583</v>
+        <v>11706540</v>
       </c>
       <c r="T14">
-        <v>57629970</v>
-      </c>
-      <c r="U14">
-        <v>100</v>
-      </c>
-      <c r="V14">
-        <v>500848235725730</v>
-      </c>
-      <c r="W14">
-        <v>500848249776562</v>
-      </c>
-      <c r="X14" s="6">
+        <v>144908396</v>
+      </c>
+      <c r="U14" s="4">
+        <v>267573724729531</v>
+      </c>
+      <c r="V14" s="4">
+        <v>267573865918403</v>
+      </c>
+      <c r="W14" s="4">
         <f t="shared" si="0"/>
-        <v>14050832</v>
-      </c>
-      <c r="Y14">
+        <v>141188872</v>
+      </c>
+      <c r="X14">
         <f t="shared" si="1"/>
-        <v>1.4050832000000001E-2</v>
+        <v>0.14118887200000002</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1470</v>
+        <v>1628</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>1569</v>
+        <v>474</v>
       </c>
       <c r="F15">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G15">
-        <v>756446</v>
+        <v>388997</v>
       </c>
       <c r="H15">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I15">
         <v>256</v>
@@ -2098,77 +2053,74 @@
         <v>28160</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L15">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M15">
         <v>112</v>
       </c>
       <c r="N15">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O15" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" t="s">
         <v>23</v>
       </c>
-      <c r="P15" t="s">
-        <v>24</v>
-      </c>
       <c r="Q15">
-        <v>1669033</v>
+        <v>11924065</v>
       </c>
       <c r="R15">
-        <v>1035889131</v>
+        <v>7460634360</v>
       </c>
       <c r="S15">
-        <v>1393620</v>
+        <v>11736527</v>
       </c>
       <c r="T15">
-        <v>57644216</v>
-      </c>
-      <c r="U15">
-        <v>100</v>
-      </c>
-      <c r="V15">
-        <v>500848406407654</v>
-      </c>
-      <c r="W15">
-        <v>500848420498644</v>
-      </c>
-      <c r="X15" s="6">
+        <v>144842468</v>
+      </c>
+      <c r="U15" s="4">
+        <v>267574540030736</v>
+      </c>
+      <c r="V15" s="4">
+        <v>267574681393359</v>
+      </c>
+      <c r="W15" s="4">
         <f t="shared" si="0"/>
-        <v>14090990</v>
-      </c>
-      <c r="Y15">
+        <v>141362623</v>
+      </c>
+      <c r="X15">
         <f t="shared" si="1"/>
-        <v>1.4090990000000001E-2</v>
+        <v>0.14136262300000002</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1854</v>
+        <v>2064</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>598</v>
+        <v>675</v>
       </c>
       <c r="F16">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G16">
-        <v>756457</v>
+        <v>388994</v>
       </c>
       <c r="H16">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I16">
         <v>256</v>
@@ -2177,59 +2129,56 @@
         <v>28160</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L16">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M16">
         <v>112</v>
       </c>
       <c r="N16">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" t="s">
         <v>23</v>
       </c>
-      <c r="P16" t="s">
-        <v>24</v>
-      </c>
       <c r="Q16">
-        <v>1668971</v>
+        <v>11890828</v>
       </c>
       <c r="R16">
-        <v>1035927442</v>
+        <v>7461347795</v>
       </c>
       <c r="S16">
-        <v>1393691</v>
+        <v>11728254</v>
       </c>
       <c r="T16">
-        <v>57645806</v>
-      </c>
-      <c r="U16">
-        <v>100</v>
-      </c>
-      <c r="V16">
-        <v>500848577403446</v>
-      </c>
-      <c r="W16">
-        <v>500848591547876</v>
-      </c>
-      <c r="X16" s="6">
+        <v>145165719</v>
+      </c>
+      <c r="U16" s="4">
+        <v>267575283608673</v>
+      </c>
+      <c r="V16" s="4">
+        <v>267575445252131</v>
+      </c>
+      <c r="W16" s="4">
         <f t="shared" si="0"/>
-        <v>14144430</v>
-      </c>
-      <c r="Y16">
+        <v>161643458</v>
+      </c>
+      <c r="X16">
         <f t="shared" si="1"/>
-        <v>1.4144430000000001E-2</v>
+        <v>0.16164345800000002</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2238</v>
+        <v>2501</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2238,16 +2187,16 @@
         <v>2</v>
       </c>
       <c r="E17">
-        <v>1958</v>
+        <v>2224</v>
       </c>
       <c r="F17">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G17">
-        <v>756455</v>
+        <v>388986</v>
       </c>
       <c r="H17">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I17">
         <v>256</v>
@@ -2256,59 +2205,56 @@
         <v>28160</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L17">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M17">
         <v>112</v>
       </c>
       <c r="N17">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O17" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" t="s">
         <v>23</v>
       </c>
-      <c r="P17" t="s">
-        <v>24</v>
-      </c>
       <c r="Q17">
-        <v>1669081</v>
+        <v>11864866</v>
       </c>
       <c r="R17">
-        <v>1035909544</v>
+        <v>7461022128</v>
       </c>
       <c r="S17">
-        <v>1393703</v>
+        <v>11697496</v>
       </c>
       <c r="T17">
-        <v>57643942</v>
-      </c>
-      <c r="U17">
-        <v>100</v>
-      </c>
-      <c r="V17">
-        <v>500848749758495</v>
-      </c>
-      <c r="W17">
-        <v>500848763931404</v>
-      </c>
-      <c r="X17" s="6">
+        <v>144796678</v>
+      </c>
+      <c r="U17" s="4">
+        <v>267576083887037</v>
+      </c>
+      <c r="V17" s="4">
+        <v>267576225620702</v>
+      </c>
+      <c r="W17" s="4">
         <f t="shared" si="0"/>
-        <v>14172909</v>
-      </c>
-      <c r="Y17">
+        <v>141733665</v>
+      </c>
+      <c r="X17">
         <f t="shared" si="1"/>
-        <v>1.4172909000000001E-2</v>
+        <v>0.14173366500000001</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2622</v>
+        <v>2938</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2317,16 +2263,16 @@
         <v>4</v>
       </c>
       <c r="E18">
-        <v>985</v>
+        <v>1122</v>
       </c>
       <c r="F18">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G18">
-        <v>756453</v>
+        <v>388997</v>
       </c>
       <c r="H18">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I18">
         <v>256</v>
@@ -2335,77 +2281,74 @@
         <v>28160</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L18">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M18">
         <v>112</v>
       </c>
       <c r="N18">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O18" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" t="s">
         <v>23</v>
       </c>
-      <c r="P18" t="s">
-        <v>24</v>
-      </c>
       <c r="Q18">
-        <v>1669042</v>
+        <v>11763543</v>
       </c>
       <c r="R18">
-        <v>1035909694</v>
+        <v>7461031649</v>
       </c>
       <c r="S18">
-        <v>1393646</v>
+        <v>11861843</v>
       </c>
       <c r="T18">
-        <v>57646392</v>
-      </c>
-      <c r="U18">
-        <v>100</v>
-      </c>
-      <c r="V18">
-        <v>500848956816426</v>
-      </c>
-      <c r="W18">
-        <v>500848971008537</v>
-      </c>
-      <c r="X18" s="6">
+        <v>145155754</v>
+      </c>
+      <c r="U18" s="4">
+        <v>267576874322931</v>
+      </c>
+      <c r="V18" s="4">
+        <v>267577040290365</v>
+      </c>
+      <c r="W18" s="4">
         <f t="shared" si="0"/>
-        <v>14192111</v>
-      </c>
-      <c r="Y18">
+        <v>165967434</v>
+      </c>
+      <c r="X18">
         <f t="shared" si="1"/>
-        <v>1.4192111E-2</v>
+        <v>0.165967434</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>3007</v>
+        <v>3374</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>2328</v>
+        <v>1304</v>
       </c>
       <c r="F19">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G19">
-        <v>756446</v>
+        <v>388994</v>
       </c>
       <c r="H19">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I19">
         <v>256</v>
@@ -2414,77 +2357,74 @@
         <v>28160</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L19">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M19">
         <v>112</v>
       </c>
       <c r="N19">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O19" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" t="s">
         <v>23</v>
       </c>
-      <c r="P19" t="s">
-        <v>24</v>
-      </c>
       <c r="Q19">
-        <v>1669081</v>
+        <v>11732343</v>
       </c>
       <c r="R19">
-        <v>1035900856</v>
+        <v>7461057497</v>
       </c>
       <c r="S19">
-        <v>1393657</v>
+        <v>11688796</v>
       </c>
       <c r="T19">
-        <v>57647900</v>
-      </c>
-      <c r="U19">
-        <v>100</v>
-      </c>
-      <c r="V19">
-        <v>500849135433271</v>
-      </c>
-      <c r="W19">
-        <v>500849149633382</v>
-      </c>
-      <c r="X19" s="6">
+        <v>144809646</v>
+      </c>
+      <c r="U19" s="4">
+        <v>267577759037135</v>
+      </c>
+      <c r="V19" s="4">
+        <v>267577900968396</v>
+      </c>
+      <c r="W19" s="4">
         <f t="shared" si="0"/>
-        <v>14200111</v>
-      </c>
-      <c r="Y19">
+        <v>141931261</v>
+      </c>
+      <c r="X19">
         <f t="shared" si="1"/>
-        <v>1.4200111000000001E-2</v>
+        <v>0.141931261</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>3391</v>
+        <v>3810</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>1353</v>
+        <v>1531</v>
       </c>
       <c r="F20">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G20">
-        <v>756457</v>
+        <v>388998</v>
       </c>
       <c r="H20">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I20">
         <v>256</v>
@@ -2493,59 +2433,56 @@
         <v>28160</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L20">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M20">
         <v>112</v>
       </c>
       <c r="N20">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" t="s">
         <v>23</v>
       </c>
-      <c r="P20" t="s">
-        <v>24</v>
-      </c>
       <c r="Q20">
-        <v>1669015</v>
+        <v>11776642</v>
       </c>
       <c r="R20">
-        <v>1035939337</v>
+        <v>7460729396</v>
       </c>
       <c r="S20">
-        <v>1393652</v>
+        <v>11710597</v>
       </c>
       <c r="T20">
-        <v>57647664</v>
-      </c>
-      <c r="U20">
-        <v>100</v>
-      </c>
-      <c r="V20">
-        <v>500849307924325</v>
-      </c>
-      <c r="W20">
-        <v>500849322130356</v>
-      </c>
-      <c r="X20" s="6">
+        <v>144720940</v>
+      </c>
+      <c r="U20" s="4">
+        <v>267578626176357</v>
+      </c>
+      <c r="V20" s="4">
+        <v>267578789848125</v>
+      </c>
+      <c r="W20" s="4">
         <f t="shared" si="0"/>
-        <v>14206031</v>
-      </c>
-      <c r="Y20">
+        <v>163671768</v>
+      </c>
+      <c r="X20">
         <f t="shared" si="1"/>
-        <v>1.4206031000000001E-2</v>
+        <v>0.16367176800000002</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>3776</v>
+        <v>4247</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2554,16 +2491,16 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>774</v>
+        <v>864</v>
       </c>
       <c r="F21">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G21">
-        <v>756456</v>
+        <v>388996</v>
       </c>
       <c r="H21">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I21">
         <v>256</v>
@@ -2572,59 +2509,56 @@
         <v>28160</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L21">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M21">
         <v>112</v>
       </c>
       <c r="N21">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O21" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" t="s">
         <v>23</v>
       </c>
-      <c r="P21" t="s">
-        <v>24</v>
-      </c>
       <c r="Q21">
-        <v>1669096</v>
+        <v>11837331</v>
       </c>
       <c r="R21">
-        <v>1035934348</v>
+        <v>7461051897</v>
       </c>
       <c r="S21">
-        <v>1393632</v>
+        <v>11761021</v>
       </c>
       <c r="T21">
-        <v>57644770</v>
-      </c>
-      <c r="U21">
-        <v>100</v>
-      </c>
-      <c r="V21">
-        <v>500849525545411</v>
-      </c>
-      <c r="W21">
-        <v>500849539777522</v>
-      </c>
-      <c r="X21" s="6">
+        <v>144831740</v>
+      </c>
+      <c r="U21" s="4">
+        <v>267579468145052</v>
+      </c>
+      <c r="V21" s="4">
+        <v>267579610310232</v>
+      </c>
+      <c r="W21" s="4">
         <f t="shared" si="0"/>
-        <v>14232111</v>
-      </c>
-      <c r="Y21">
+        <v>142165180</v>
+      </c>
+      <c r="X21">
         <f t="shared" si="1"/>
-        <v>1.4232111E-2</v>
+        <v>0.14216518</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>4161</v>
+        <v>4685</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2633,16 +2567,16 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>2886</v>
+        <v>3292</v>
       </c>
       <c r="F22">
-        <v>756432</v>
+        <v>388975</v>
       </c>
       <c r="G22">
-        <v>756455</v>
+        <v>388995</v>
       </c>
       <c r="H22">
-        <v>2097152</v>
+        <v>14622720</v>
       </c>
       <c r="I22">
         <v>256</v>
@@ -2651,93 +2585,88 @@
         <v>28160</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L22">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M22">
         <v>112</v>
       </c>
       <c r="N22">
-        <v>126528</v>
+        <v>126464</v>
       </c>
       <c r="O22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" t="s">
         <v>23</v>
       </c>
-      <c r="P22" t="s">
-        <v>24</v>
-      </c>
       <c r="Q22">
-        <v>1669109</v>
+        <v>11758002</v>
       </c>
       <c r="R22">
-        <v>1035965606</v>
+        <v>7460139643</v>
       </c>
       <c r="S22">
-        <v>1393655</v>
+        <v>11729125</v>
       </c>
       <c r="T22">
-        <v>57647164</v>
-      </c>
-      <c r="U22">
-        <v>100</v>
-      </c>
-      <c r="V22">
-        <v>500849703598297</v>
-      </c>
-      <c r="W22">
-        <v>500849717834248</v>
-      </c>
-      <c r="X22" s="6">
+        <v>144792730</v>
+      </c>
+      <c r="U22" s="4">
+        <v>267580288660610</v>
+      </c>
+      <c r="V22" s="4">
+        <v>267580457092183</v>
+      </c>
+      <c r="W22" s="4">
         <f t="shared" si="0"/>
-        <v>14235951</v>
-      </c>
-      <c r="Y22">
+        <v>168431573</v>
+      </c>
+      <c r="X22">
         <f t="shared" si="1"/>
-        <v>1.4235951E-2</v>
+        <v>0.168431573</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q23" s="3">
-        <f>AVERAGE(Q13:Q22)</f>
-        <v>1668848.5</v>
+        <f>MAX(Q13:Q22)</f>
+        <v>11924065</v>
       </c>
       <c r="R23" s="3">
-        <f>AVERAGE(R13:R22)</f>
-        <v>1035404225.8</v>
+        <f t="shared" ref="R23:T23" si="3">MAX(R13:R22)</f>
+        <v>7461347795</v>
       </c>
       <c r="S23" s="3">
-        <f>AVERAGE(S13:S22)</f>
-        <v>1393230.2</v>
+        <f t="shared" si="3"/>
+        <v>11861843</v>
       </c>
       <c r="T23" s="3">
-        <f>AVERAGE(T13:T22)</f>
-        <v>57614951.200000003</v>
-      </c>
-      <c r="U23" s="4">
-        <f>AVERAGE(U13:U22)</f>
-        <v>100</v>
-      </c>
-      <c r="X23" s="4">
-        <f>AVERAGE(X13:X22)</f>
-        <v>14127310.6</v>
-      </c>
-      <c r="Y23" s="3">
-        <f t="shared" ref="Y23" si="2">X23 * POWER(10, -9)</f>
-        <v>1.41273106E-2</v>
+        <f t="shared" si="3"/>
+        <v>145895567</v>
+      </c>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5">
+        <f>AVERAGE(W13:W22)</f>
+        <v>152873721.5</v>
+      </c>
+      <c r="X23" s="3">
+        <f t="shared" si="1"/>
+        <v>0.1528737215</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V22">
     <sortCondition ref="B2:B22"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="X12" formula="1"/>
+    <ignoredError sqref="W12" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>